<commit_message>
Auto commit at 2025-10-08  9:06:29.72
</commit_message>
<xml_diff>
--- a/comprehensivedata/202509-202509.xlsx
+++ b/comprehensivedata/202509-202509.xlsx
@@ -116,7 +116,7 @@
   </si>
   <si>
     <t xml:space="preserve">单位：长沙飞狐电动汽车充电服务有限公司                                                                                             </t>
-    <phoneticPr fontId="20" type="noConversion"/>
+    <phoneticPr fontId="21" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -124,15 +124,23 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
-    <numFmt numFmtId="181" formatCode="0.00_ "/>
+    <numFmt numFmtId="176" formatCode="0.00_);[Red]\(0.00\)"/>
+    <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -716,54 +724,140 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="45">
+  <cellStyleXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -772,7 +866,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -781,7 +875,7 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -790,7 +884,7 @@
     <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -799,7 +893,7 @@
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -808,7 +902,7 @@
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -817,145 +911,137 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="34" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="13" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="45" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="13" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="11" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="34" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="12" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="34" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="13" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="34" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="34" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="12" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="11" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="17" xfId="34" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="34" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="34" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="34">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="34" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="10" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="34" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="17" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="34" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="10" xfId="34" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="10" xfId="34" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="19" fillId="0" borderId="10" xfId="34" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="19" fillId="34" borderId="10" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="19" fillId="34" borderId="10" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="19" fillId="35" borderId="13" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="19" fillId="34" borderId="10" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="181" fontId="19" fillId="35" borderId="10" xfId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="45" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="20" fillId="34" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="20" fillId="34" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="20" fillId="35" borderId="13" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="20" fillId="34" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="20" fillId="35" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="45">
+  <cellStyles count="65">
     <cellStyle name="20% - 着色 1" xfId="17" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 1 2" xfId="47"/>
     <cellStyle name="20% - 着色 2" xfId="20" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 2 2" xfId="50"/>
     <cellStyle name="20% - 着色 3" xfId="23" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 3 2" xfId="53"/>
     <cellStyle name="20% - 着色 4" xfId="26" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 4 2" xfId="56"/>
     <cellStyle name="20% - 着色 5" xfId="29" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 5 2" xfId="59"/>
     <cellStyle name="20% - 着色 6" xfId="32" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - 着色 6 2" xfId="62"/>
     <cellStyle name="40% - 着色 1" xfId="18" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 1 2" xfId="48"/>
     <cellStyle name="40% - 着色 2" xfId="21" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 2 2" xfId="51"/>
     <cellStyle name="40% - 着色 3" xfId="24" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 3 2" xfId="54"/>
     <cellStyle name="40% - 着色 4" xfId="27" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 4 2" xfId="57"/>
     <cellStyle name="40% - 着色 5" xfId="30" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 5 2" xfId="60"/>
     <cellStyle name="40% - 着色 6" xfId="33" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - 着色 6 2" xfId="63"/>
     <cellStyle name="60% - 着色 1 2" xfId="38"/>
+    <cellStyle name="60% - 着色 1 3" xfId="49"/>
     <cellStyle name="60% - 着色 2 2" xfId="39"/>
+    <cellStyle name="60% - 着色 2 3" xfId="52"/>
     <cellStyle name="60% - 着色 3 2" xfId="40"/>
+    <cellStyle name="60% - 着色 3 3" xfId="55"/>
     <cellStyle name="60% - 着色 4 2" xfId="41"/>
+    <cellStyle name="60% - 着色 4 3" xfId="58"/>
     <cellStyle name="60% - 着色 5 2" xfId="42"/>
+    <cellStyle name="60% - 着色 5 3" xfId="61"/>
     <cellStyle name="60% - 着色 6 2" xfId="43"/>
+    <cellStyle name="60% - 着色 6 3" xfId="64"/>
     <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
@@ -966,6 +1052,7 @@
     <cellStyle name="常规 2" xfId="35"/>
     <cellStyle name="常规 3" xfId="44"/>
     <cellStyle name="常规 4" xfId="34"/>
+    <cellStyle name="常规 5" xfId="45"/>
     <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="汇总" xfId="15" builtinId="25" customBuiltin="1"/>
     <cellStyle name="计算" xfId="10" builtinId="22" customBuiltin="1"/>
@@ -983,6 +1070,7 @@
     <cellStyle name="着色 5" xfId="28" builtinId="45" customBuiltin="1"/>
     <cellStyle name="着色 6" xfId="31" builtinId="49" customBuiltin="1"/>
     <cellStyle name="注释 2" xfId="37"/>
+    <cellStyle name="注释 3" xfId="46"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -1287,7 +1375,7 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1298,102 +1386,102 @@
     <col min="8" max="8" width="7.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="5.25" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.625" bestFit="1" customWidth="1"/>
     <col min="16" max="17" width="12" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
     </row>
-    <row r="2" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="13" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
     </row>
-    <row r="3" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="14" t="s">
+    <row r="3" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="7" t="s">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="9" t="s">
         <v>5</v>
       </c>
       <c r="I3" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14" t="s">
+      <c r="K3" s="13"/>
+      <c r="L3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14" t="s">
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="1" t="s">
+      <c r="Q3" s="13"/>
+      <c r="R3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="9" t="s">
+      <c r="S3" s="8" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="14"/>
+    <row r="4" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="13"/>
       <c r="B4" s="20" t="s">
         <v>12</v>
       </c>
@@ -1409,8 +1497,8 @@
       <c r="F4" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
       <c r="I4" s="17" t="s">
         <v>17</v>
       </c>
@@ -1438,10 +1526,10 @@
       <c r="Q4" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="10"/>
-      <c r="S4" s="9"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="8"/>
     </row>
-    <row r="5" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="17" t="s">
         <v>25</v>
       </c>
@@ -1451,13 +1539,13 @@
       <c r="C5" s="17">
         <v>374.52</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="9">
         <v>-330.74</v>
       </c>
-      <c r="E5" s="7">
+      <c r="E5" s="9">
         <v>2702</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="9">
         <v>-90</v>
       </c>
       <c r="G5" s="17">
@@ -1484,7 +1572,7 @@
         <v>12195.869999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="17" t="s">
         <v>26</v>
       </c>
@@ -1494,9 +1582,9 @@
       <c r="C6" s="17">
         <v>340.3</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17"/>
@@ -1517,7 +1605,7 @@
         <v>11735.75</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>27</v>
       </c>
@@ -1527,9 +1615,9 @@
       <c r="C7" s="17">
         <v>350.1</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
@@ -1550,17 +1638,17 @@
         <v>6516.91</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="18" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="4">
         <v>4308.03</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="8"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="18">
         <v>1580</v>
       </c>
@@ -1589,15 +1677,15 @@
         <v>30448.53</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="18" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="4"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="8"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="22"/>
       <c r="H9" s="28"/>
       <c r="I9" s="18">
@@ -1615,16 +1703,20 @@
       <c r="M9" s="18">
         <v>6726</v>
       </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
+      <c r="N9" s="18">
+        <v>3617.25</v>
+      </c>
+      <c r="O9" s="18">
+        <v>1260.27</v>
+      </c>
       <c r="P9" s="18"/>
       <c r="Q9" s="18"/>
       <c r="R9" s="18"/>
       <c r="S9" s="18">
-        <v>8859.6</v>
+        <v>11298.359999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="36.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="19" t="s">
         <v>30</v>
       </c>
@@ -1649,7 +1741,7 @@
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="12">
-        <v>6585</v>
+        <v>9023.76</v>
       </c>
       <c r="M10" s="11"/>
       <c r="N10" s="11"/>
@@ -1662,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="S10" s="19">
-        <v>39308.129999999997</v>
+        <v>41746.89</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
@@ -1688,9 +1780,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="J10:K10"/>
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="L10:O10"/>
@@ -1709,8 +1798,11 @@
     <mergeCell ref="P3:Q3"/>
     <mergeCell ref="P2:S2"/>
     <mergeCell ref="A2:O2"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="J10:K10"/>
   </mergeCells>
-  <phoneticPr fontId="20" type="noConversion"/>
+  <phoneticPr fontId="21" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Auto commit at 2025-10-09 10:20:08.49
</commit_message>
<xml_diff>
--- a/comprehensivedata/202509-202509.xlsx
+++ b/comprehensivedata/202509-202509.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -917,92 +917,92 @@
   </cellStyleXfs>
   <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="45" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="20" fillId="0" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="20" fillId="34" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="20" fillId="34" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="20" fillId="35" borderId="13" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="20" fillId="34" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="20" fillId="35" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="13" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="17" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="12" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="13" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="13" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="45" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="12" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="45" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="20" fillId="0" borderId="17" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="45" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="45" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="10" xfId="45" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="10" xfId="45" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="20" fillId="0" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="20" fillId="34" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="20" fillId="34" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="20" fillId="35" borderId="13" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="20" fillId="34" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="20" fillId="35" borderId="10" xfId="45" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="65">
@@ -1372,10 +1372,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1392,394 +1393,402 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
     </row>
     <row r="2" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="15" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
+      <c r="Q2" s="28"/>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
     </row>
     <row r="3" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="9" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="13" t="s">
+      <c r="J3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13" t="s">
+      <c r="K3" s="27"/>
+      <c r="L3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="M3" s="13"/>
-      <c r="N3" s="13"/>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13" t="s">
+      <c r="M3" s="27"/>
+      <c r="N3" s="27"/>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="10" t="s">
+      <c r="Q3" s="27"/>
+      <c r="R3" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="13"/>
-      <c r="B4" s="20" t="s">
+      <c r="A4" s="27"/>
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="17" t="s">
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="J4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K4" s="17" t="s">
+      <c r="K4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="20" t="s">
+      <c r="L4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="20" t="s">
+      <c r="M4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="17" t="s">
+      <c r="O4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="P4" s="17" t="s">
+      <c r="P4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="17" t="s">
+      <c r="Q4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="R4" s="5"/>
-      <c r="S4" s="8"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="17"/>
     </row>
     <row r="5" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="2">
         <v>630.85</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="2">
         <v>374.52</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="19">
         <v>-330.74</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="19">
         <v>2702</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="19">
         <v>-90</v>
       </c>
-      <c r="G5" s="17">
+      <c r="G5" s="2">
         <v>1580</v>
       </c>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17">
+      <c r="H5" s="2"/>
+      <c r="I5" s="2">
         <v>2695.5</v>
       </c>
-      <c r="J5" s="17"/>
-      <c r="K5" s="17"/>
-      <c r="L5" s="17"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="23">
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="8">
         <v>3895</v>
       </c>
-      <c r="Q5" s="23">
+      <c r="Q5" s="8">
         <v>3020</v>
       </c>
-      <c r="R5" s="23"/>
-      <c r="S5" s="24">
+      <c r="R5" s="8"/>
+      <c r="S5" s="9">
         <v>12195.869999999999</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="2">
         <v>139.19</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="2">
         <v>340.3</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="23">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="8">
         <v>4175</v>
       </c>
-      <c r="Q6" s="23">
+      <c r="Q6" s="8">
         <v>4800</v>
       </c>
-      <c r="R6" s="23"/>
-      <c r="S6" s="24">
+      <c r="R6" s="8"/>
+      <c r="S6" s="9">
         <v>11735.75</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="17">
+      <c r="B7" s="2">
         <v>191.81</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="2">
         <v>350.1</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
-      <c r="P7" s="23">
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="8">
         <v>3255</v>
       </c>
-      <c r="Q7" s="23">
+      <c r="Q7" s="8">
         <v>2720</v>
       </c>
-      <c r="R7" s="23"/>
-      <c r="S7" s="24">
+      <c r="R7" s="8"/>
+      <c r="S7" s="9">
         <v>6516.91</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="22">
         <v>4308.03</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="18">
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="3">
         <v>1580</v>
       </c>
-      <c r="H8" s="26">
+      <c r="H8" s="11">
         <v>0</v>
       </c>
-      <c r="I8" s="18">
+      <c r="I8" s="3">
         <v>2695.5</v>
       </c>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="25">
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="10">
         <v>11325</v>
       </c>
-      <c r="Q8" s="26">
+      <c r="Q8" s="11">
         <v>10540</v>
       </c>
-      <c r="R8" s="26">
+      <c r="R8" s="11">
         <v>0</v>
       </c>
-      <c r="S8" s="25">
+      <c r="S8" s="10">
         <v>30448.53</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="18">
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="3">
         <v>1054.3</v>
       </c>
-      <c r="J9" s="18">
+      <c r="J9" s="3">
         <v>680.3</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="3">
         <v>540</v>
       </c>
-      <c r="L9" s="18">
+      <c r="L9" s="3">
         <v>6444</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="3">
         <v>6726</v>
       </c>
-      <c r="N9" s="18">
-        <v>3617.25</v>
-      </c>
-      <c r="O9" s="18">
+      <c r="N9" s="3">
+        <v>3620.18</v>
+      </c>
+      <c r="O9" s="3">
         <v>1260.27</v>
       </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18">
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3">
         <v>11298.359999999999</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="15">
         <v>4308.03</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="19">
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="4">
         <v>1580</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H10" s="14">
         <v>0</v>
       </c>
-      <c r="I10" s="19">
+      <c r="I10" s="4">
         <v>3749.8</v>
       </c>
-      <c r="J10" s="12">
+      <c r="J10" s="15">
         <v>1220.3</v>
       </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="12">
-        <v>9023.76</v>
-      </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="12">
+      <c r="K10" s="16"/>
+      <c r="L10" s="15">
+        <v>9025.2199999999993</v>
+      </c>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="15">
         <v>21865</v>
       </c>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="27">
+      <c r="Q10" s="16"/>
+      <c r="R10" s="12">
         <v>0</v>
       </c>
-      <c r="S10" s="19">
+      <c r="S10" s="4">
         <v>41746.89</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A14" s="16"/>
-      <c r="B14" s="16"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="16"/>
-      <c r="H14" s="16"/>
-      <c r="I14" s="16"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="16"/>
-      <c r="L14" s="16"/>
-      <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="16"/>
-      <c r="R14" s="16"/>
-      <c r="S14" s="16"/>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="L3:O3"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="P2:S2"/>
+    <mergeCell ref="A2:O2"/>
     <mergeCell ref="P10:Q10"/>
     <mergeCell ref="S3:S4"/>
     <mergeCell ref="L10:O10"/>
@@ -1790,14 +1799,6 @@
     <mergeCell ref="R3:R4"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="H3:H4"/>
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="L3:O3"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="P2:S2"/>
-    <mergeCell ref="A2:O2"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="J10:K10"/>

</xml_diff>